<commit_message>
multiple prof per assignment implemented but hashable problem is accruing
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44002E7-4FC7-41EC-A633-BB6866FD47A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8EF9B7-9FBA-4C41-B645-EB80471168A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9315" yWindow="2250" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="172">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -450,30 +450,6 @@
     <t>TP</t>
   </si>
   <si>
-    <t>Mechaoui</t>
-  </si>
-  <si>
-    <t>Miroud</t>
-  </si>
-  <si>
-    <t>Bessaoud</t>
-  </si>
-  <si>
-    <t>Merafoul</t>
-  </si>
-  <si>
-    <t>Midoun</t>
-  </si>
-  <si>
-    <t>Kenniche</t>
-  </si>
-  <si>
-    <t>Bahnes</t>
-  </si>
-  <si>
-    <t>Mohammedi</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -541,6 +517,33 @@
   </si>
   <si>
     <t>capacity</t>
+  </si>
+  <si>
+    <t>Mechaoui(*)</t>
+  </si>
+  <si>
+    <t>Bessaoud(*)</t>
+  </si>
+  <si>
+    <t>Merafoul(*)</t>
+  </si>
+  <si>
+    <t>Kenniche(*)</t>
+  </si>
+  <si>
+    <t>Bahnes(*)</t>
+  </si>
+  <si>
+    <t>Mohammedi(*)</t>
+  </si>
+  <si>
+    <t>Midoun(*)</t>
+  </si>
+  <si>
+    <t>Miroud(*)</t>
+  </si>
+  <si>
+    <t>Mohammedi(2,3,4,5,6,7),medame(1)</t>
   </si>
 </sst>
 </file>
@@ -2053,16 +2056,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEAB688-FE2C-4D71-BC29-A31A67E4BF5E}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,13 +2087,13 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,13 +2101,13 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,13 +2115,13 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,10 +2129,10 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,10 +2140,10 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,10 +2151,10 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,7 +2162,7 @@
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19893C-3433-4E5A-B231-F0E5406405D5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2179,18 +2182,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -2201,7 +2204,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2212,7 +2215,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2223,7 +2226,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -2234,7 +2237,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2245,7 +2248,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2256,7 +2259,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -2267,7 +2270,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2289,7 +2292,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2300,7 +2303,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2311,7 +2314,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2337,15 +2340,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -2353,7 +2356,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -2369,7 +2372,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -2377,7 +2380,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -2385,7 +2388,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -2393,7 +2396,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B8">
         <v>21</v>

</xml_diff>

<commit_message>
multiple prof per assignment working now
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8EF9B7-9FBA-4C41-B645-EB80471168A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FF5BF9-B249-4D69-A7D4-51855E719B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
+    <workbookView xWindow="1545" yWindow="2265" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="165">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -493,27 +493,6 @@
   </si>
   <si>
     <t>groups</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>G5</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>G7</t>
   </si>
   <si>
     <t>capacity</t>
@@ -2056,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEAB688-FE2C-4D71-BC29-A31A67E4BF5E}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,13 +2066,13 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
         <v>163</v>
       </c>
-      <c r="C2" t="s">
-        <v>170</v>
-      </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,13 +2080,13 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,13 +2094,13 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,10 +2108,10 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,10 +2119,10 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2151,10 +2130,10 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,7 +2141,7 @@
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2332,8 +2311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8811BF-08BF-4B4B-A1A4-780FC5698012}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,60 +2322,60 @@
         <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>155</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>156</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>157</v>
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>158</v>
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>159</v>
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>160</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>161</v>
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8">
         <v>21</v>

</xml_diff>

<commit_message>
final commit before multiPromo
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3091F2D0-E8B9-45C8-81F7-FFDE42CCCB49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D7E067-94EA-41E7-83DE-D56146183AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="165">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -2151,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19893C-3433-4E5A-B231-F0E5406405D5}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -2282,23 +2282,12 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
multiPromo supported and excel exporter rewrite
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D7E067-94EA-41E7-83DE-D56146183AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFF4FC4-693D-4165-B999-B170BF567616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
     <sheet name="Professors" sheetId="3" r:id="rId2"/>
     <sheet name="Rooms" sheetId="4" r:id="rId3"/>
-    <sheet name="L3" sheetId="5" r:id="rId4"/>
+    <sheet name="Promos" sheetId="6" r:id="rId4"/>
+    <sheet name="L3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="325">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -117,9 +118,6 @@
     <t xml:space="preserve">UET211 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Physique 2 (électricité générale)</t>
-  </si>
-  <si>
     <t>UEF311</t>
   </si>
   <si>
@@ -432,12 +430,6 @@
     <t>Nb_TP</t>
   </si>
   <si>
-    <t>Coeff</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -483,9 +475,6 @@
     <t>Amphi4</t>
   </si>
   <si>
-    <t>S03</t>
-  </si>
-  <si>
     <t>S16</t>
   </si>
   <si>
@@ -523,13 +512,505 @@
   </si>
   <si>
     <t>Mohammedi(2,3,4,5,6,7),medame(1)</t>
+  </si>
+  <si>
+    <t>Promo</t>
+  </si>
+  <si>
+    <t>nb_section</t>
+  </si>
+  <si>
+    <t>nb_group</t>
+  </si>
+  <si>
+    <t>nb_etd</t>
+  </si>
+  <si>
+    <t>TC-MI</t>
+  </si>
+  <si>
+    <t>L2-INFO</t>
+  </si>
+  <si>
+    <t>L3-INFO</t>
+  </si>
+  <si>
+    <t>L2-MATH</t>
+  </si>
+  <si>
+    <t>L3-MATH</t>
+  </si>
+  <si>
+    <t>prof_cour</t>
+  </si>
+  <si>
+    <t>prof_td</t>
+  </si>
+  <si>
+    <t>prof_tp</t>
+  </si>
+  <si>
+    <t>BENIDRIS(7)</t>
+  </si>
+  <si>
+    <t>M. Ould Ali M(2),Mme Ablaoui(2),Mme Bendehmane H(2),M. Kaid(4),Mlle FERRAOUN A.(2),Mlle Bouabdelli(2)</t>
+  </si>
+  <si>
+    <t>M. Medeghri Ahmed(2)</t>
+  </si>
+  <si>
+    <t>Mme TABHARIT(5),Mme SAIDANI(4),Mme Diala.H(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Physique 2(électricité générale)</t>
+  </si>
+  <si>
+    <t>MECHAOUI(7)</t>
+  </si>
+  <si>
+    <t>HOCINE(7)</t>
+  </si>
+  <si>
+    <t>DELALI(7)</t>
+  </si>
+  <si>
+    <t>SEHABA(5),HENNI K(4)</t>
+  </si>
+  <si>
+    <t>ABID(6),BETOUATI(3)</t>
+  </si>
+  <si>
+    <t>LAREDJ(3),BOUZEBIBA(6)</t>
+  </si>
+  <si>
+    <t>BENHAMED(7), MOUSSA(2)</t>
+  </si>
+  <si>
+    <t>BESSAOUD(3),BESNASSI(3),MIDOUN(3)</t>
+  </si>
+  <si>
+    <t>KENNICHE(3),DJAHAFI(3),HENNI K(3)</t>
+  </si>
+  <si>
+    <t>MIROUD(3),BETOUATI(4),MEROUFEL(2)</t>
+  </si>
+  <si>
+    <t>MECHAOUI M. D.G(1)</t>
+  </si>
+  <si>
+    <t>BENIDRIS F.Z(1)</t>
+  </si>
+  <si>
+    <t>HOCINE N.(1)</t>
+  </si>
+  <si>
+    <t>DELALI A.(1)</t>
+  </si>
+  <si>
+    <t>MIDOUN M.(1)</t>
+  </si>
+  <si>
+    <t>HENNI F(1),KAID SLIMANE(3),BENSALLOUA(4),BENAMEUR(3),MOUMEN(1),Zahmani(2)</t>
+  </si>
+  <si>
+    <t>HENNI F(2)</t>
+  </si>
+  <si>
+    <t>HASSAINE(2)</t>
+  </si>
+  <si>
+    <t>HENNI K. (2)</t>
+  </si>
+  <si>
+    <t>BESSAOUD K.(1)</t>
+  </si>
+  <si>
+    <t>KENNICHE A.(1)</t>
+  </si>
+  <si>
+    <t>MAGHNI SANDID Z.(1)</t>
+  </si>
+  <si>
+    <t>LAREDJ A. M(1)</t>
+  </si>
+  <si>
+    <t>ABID M.(1)</t>
+  </si>
+  <si>
+    <t>SEHABA K.(1)</t>
+  </si>
+  <si>
+    <t>Mlle Dj. BENSIKADDOUR(2)</t>
+  </si>
+  <si>
+    <t>Mlle Dj. BENSIKADDOUR(1),M. Benyatou Kamel(2),Mme Kaisserli(5),M. Benzidane(2),Mlle Benaouad(2),Mlle Zelmat Souhila(2)</t>
+  </si>
+  <si>
+    <t>Mlle Ali Merina.H(2)</t>
+  </si>
+  <si>
+    <t>Mlle Ali Merina.H(4),Mlle Hamou Maamar.M(5),Mlle Bouzid(3),Mlle Lakeb Ouda(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UEF311 </t>
+  </si>
+  <si>
+    <t>Algèbre 3</t>
+  </si>
+  <si>
+    <t>Analyse 3</t>
+  </si>
+  <si>
+    <t>Introduction à la topologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UEF313 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UEM313 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D311 </t>
+  </si>
+  <si>
+    <t>Analyse numérique 1</t>
+  </si>
+  <si>
+    <t>Outils de Programmation 2</t>
+  </si>
+  <si>
+    <t>Histoire des Mathématiques</t>
+  </si>
+  <si>
+    <t>ALG3</t>
+  </si>
+  <si>
+    <t>ANA4</t>
+  </si>
+  <si>
+    <t>ANA3</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>ANUM</t>
+  </si>
+  <si>
+    <t>OPM2</t>
+  </si>
+  <si>
+    <t>HM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F411 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F412 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F413 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M411 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M412 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M413 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D411 </t>
+  </si>
+  <si>
+    <t>Analyse 4</t>
+  </si>
+  <si>
+    <t>Algèbre 4</t>
+  </si>
+  <si>
+    <t>Analyse complexe</t>
+  </si>
+  <si>
+    <t>Analyse Numérique 2</t>
+  </si>
+  <si>
+    <t>Probabilités</t>
+  </si>
+  <si>
+    <t>Géométrie</t>
+  </si>
+  <si>
+    <t>Application des mathématiques aux autres sciences</t>
+  </si>
+  <si>
+    <t>ALG4</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>ANUM2</t>
+  </si>
+  <si>
+    <t>PROBA</t>
+  </si>
+  <si>
+    <t>GÉOMÉ</t>
+  </si>
+  <si>
+    <t>APsciences</t>
+  </si>
+  <si>
+    <t>Mme Limam(1)</t>
+  </si>
+  <si>
+    <t>Mme Limam(2)</t>
+  </si>
+  <si>
+    <t>M.Ould ali(1)</t>
+  </si>
+  <si>
+    <t>M.Ould ali(2)</t>
+  </si>
+  <si>
+    <t>Mlle Amina FERRAOUN(1)</t>
+  </si>
+  <si>
+    <t>Mlle Amina FERRAOUN(2)</t>
+  </si>
+  <si>
+    <t>M. Belhamiti Omar(1)</t>
+  </si>
+  <si>
+    <t>M. Belhamiti Omar(2)</t>
+  </si>
+  <si>
+    <t>M. Mohammedi Mustapha(1)</t>
+  </si>
+  <si>
+    <t>M. Mohammedi Mustapha(2)</t>
+  </si>
+  <si>
+    <t>Mme Bendahmane Hafida(1)</t>
+  </si>
+  <si>
+    <t>M. Ghezzar Med(1)</t>
+  </si>
+  <si>
+    <t>Mesure et intégration</t>
+  </si>
+  <si>
+    <t>Espaces vectoriels normés</t>
+  </si>
+  <si>
+    <t>Equations différentielles</t>
+  </si>
+  <si>
+    <t>Equations de la physique mathématique</t>
+  </si>
+  <si>
+    <t>Optimisation sans contraintes</t>
+  </si>
+  <si>
+    <t>Initiation å la didactique des mathématiques</t>
+  </si>
+  <si>
+    <t>UEF5.1.1</t>
+  </si>
+  <si>
+    <t>UEF5.1.2</t>
+  </si>
+  <si>
+    <t>UEF5.2.1</t>
+  </si>
+  <si>
+    <t>UEF5.2.2</t>
+  </si>
+  <si>
+    <t>UEM5.1.1</t>
+  </si>
+  <si>
+    <t>UED5.1</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>EVN</t>
+  </si>
+  <si>
+    <t>EPM</t>
+  </si>
+  <si>
+    <t>OSC</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Transformations intégrales dans les espaces L</t>
+  </si>
+  <si>
+    <t>Géométrie différentielle</t>
+  </si>
+  <si>
+    <t>Ethique et déontologie de l'enseignement et de la recherche</t>
+  </si>
+  <si>
+    <t>UEF6.1.1</t>
+  </si>
+  <si>
+    <t>UEF6.1.2</t>
+  </si>
+  <si>
+    <t>UEF6.2.1</t>
+  </si>
+  <si>
+    <t>UEF6.2.2</t>
+  </si>
+  <si>
+    <t>UET6.1</t>
+  </si>
+  <si>
+    <t>TRAL</t>
+  </si>
+  <si>
+    <t>ETHrecherche</t>
+  </si>
+  <si>
+    <t>Géo. Diff</t>
+  </si>
+  <si>
+    <t>Introduction à la théorie des opérateurs linéaire</t>
+  </si>
+  <si>
+    <t>EDP</t>
+  </si>
+  <si>
+    <t>TOL</t>
+  </si>
+  <si>
+    <t>M. Andasmas(2)</t>
+  </si>
+  <si>
+    <t>M. BELARBI Lakehal(1)</t>
+  </si>
+  <si>
+    <t>M. Fettouch Houari(2)</t>
+  </si>
+  <si>
+    <t>M. Menad Abdallah(1)</t>
+  </si>
+  <si>
+    <t>M. Kaid Med(1)</t>
+  </si>
+  <si>
+    <t>Mme Belmouhoub-Ould ali(1)</t>
+  </si>
+  <si>
+    <t>Mme Belmouhoub-Ould ali(2)</t>
+  </si>
+  <si>
+    <t>M. Menad Abdallah(2)</t>
+  </si>
+  <si>
+    <t>Mme Ablaoui(1),Mr Bouzit H(1)</t>
+  </si>
+  <si>
+    <t>M. Benchehida(2)</t>
+  </si>
+  <si>
+    <t>M. Benchehida(4),Labdelli(5),Mekemmeche(5)</t>
+  </si>
+  <si>
+    <t>HASSAINE(3),HAMAMI(8),DJAHAFI(3)</t>
+  </si>
+  <si>
+    <t>KENNICHE(3),KHIAT(2),DJAHAFI(2),BOUZEBIBA(2)</t>
+  </si>
+  <si>
+    <t>MAGHNI SANDID(5),MENAD(3),MIROUD(1)</t>
+  </si>
+  <si>
+    <t>HOCINE N.(7)</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Amphi1</t>
+  </si>
+  <si>
+    <t>Amphi2</t>
+  </si>
+  <si>
+    <t>Mme Bendahmane Hafida(2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,16 +1050,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -586,11 +1079,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -632,6 +1140,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA34FF-0E82-47CA-8C99-448458D5C5EE}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="C45" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,37 +1472,41 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" customWidth="1"/>
+    <col min="9" max="9" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
       <c r="G1" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
@@ -1005,14 +1523,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="4">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1029,14 +1543,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="4">
-        <v>3</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -1055,14 +1565,10 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="4">
-        <v>4</v>
-      </c>
-      <c r="H4" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1576,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1079,14 +1585,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="4">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -1094,21 +1596,17 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -1116,21 +1614,17 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -1138,7 +1632,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1147,14 +1641,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="4">
-        <v>2</v>
-      </c>
-      <c r="H8" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1162,7 +1652,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -1171,14 +1661,14 @@
         <v>1</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="4">
-        <v>4</v>
-      </c>
-      <c r="H9" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+      <c r="H9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1676,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1195,14 +1685,14 @@
         <v>1</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="4">
-        <v>2</v>
-      </c>
-      <c r="H10" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
@@ -1210,7 +1700,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1221,14 +1711,17 @@
       <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
-        <v>4</v>
-      </c>
-      <c r="H11" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1729,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1245,14 +1738,14 @@
         <v>1</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="4">
-        <v>2</v>
-      </c>
-      <c r="H12" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
@@ -1260,7 +1753,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1269,14 +1762,14 @@
         <v>1</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
@@ -1284,21 +1777,18 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="H14" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1796,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1315,148 +1805,132 @@
       <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>205</v>
+      </c>
+      <c r="H15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" t="s">
+        <v>297</v>
+      </c>
+      <c r="H16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4">
-        <v>2</v>
-      </c>
-      <c r="H16" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="10">
-        <v>1</v>
-      </c>
-      <c r="G17" s="11">
-        <v>3</v>
-      </c>
-      <c r="H17" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D18" s="8">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="8">
-        <v>2</v>
-      </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="10">
-        <v>1</v>
-      </c>
-      <c r="G18" s="11">
-        <v>3</v>
-      </c>
-      <c r="H18" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9">
-        <v>1</v>
-      </c>
-      <c r="F19" s="10">
-        <v>1</v>
-      </c>
-      <c r="G19" s="11">
-        <v>3</v>
-      </c>
-      <c r="H19" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
         <v>104</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="11">
-        <v>2</v>
-      </c>
-      <c r="H20" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>105</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
@@ -1465,172 +1939,172 @@
       <c r="F21" s="10">
         <v>1</v>
       </c>
-      <c r="G21" s="11">
-        <v>2</v>
-      </c>
-      <c r="H21" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
         <v>106</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="11">
-        <v>2</v>
-      </c>
-      <c r="H22" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>107</v>
       </c>
       <c r="D23" s="8">
         <v>1</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H24" t="s">
+        <v>185</v>
+      </c>
+      <c r="I24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="8">
-        <v>1</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1</v>
-      </c>
-      <c r="G24" s="11">
-        <v>2</v>
-      </c>
-      <c r="H24" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" t="s">
+        <v>300</v>
+      </c>
+      <c r="I25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="8">
-        <v>1</v>
-      </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11">
-        <v>3</v>
-      </c>
-      <c r="H25" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" t="s">
+        <v>301</v>
+      </c>
+      <c r="I26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="8">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="F26" s="10">
-        <v>1</v>
-      </c>
-      <c r="G26" s="11">
-        <v>3</v>
-      </c>
-      <c r="H26" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>200</v>
+      </c>
+      <c r="H27" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>111</v>
-      </c>
-      <c r="D27" s="8">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
-      </c>
-      <c r="G27" s="11">
-        <v>3</v>
-      </c>
-      <c r="H27" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>112</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
@@ -1639,22 +2113,22 @@
       <c r="F28" s="10">
         <v>1</v>
       </c>
-      <c r="G28" s="11">
-        <v>2</v>
-      </c>
-      <c r="H28" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="8">
         <v>1</v>
@@ -1663,218 +2137,170 @@
       <c r="F29" s="10">
         <v>1</v>
       </c>
-      <c r="G29" s="11">
-        <v>2</v>
-      </c>
-      <c r="H29" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="8">
         <v>1</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="11">
-        <v>1</v>
-      </c>
-      <c r="H30" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="8">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1</v>
-      </c>
-      <c r="F31" s="10">
-        <v>1</v>
-      </c>
-      <c r="G31" s="11">
-        <v>3</v>
-      </c>
-      <c r="H31" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="8">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10">
-        <v>1</v>
-      </c>
-      <c r="G32" s="11">
-        <v>3</v>
-      </c>
-      <c r="H32" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="8">
-        <v>1</v>
-      </c>
-      <c r="E33" s="9">
-        <v>1</v>
-      </c>
-      <c r="F33" s="10">
-        <v>1</v>
-      </c>
-      <c r="G33" s="11">
-        <v>3</v>
-      </c>
-      <c r="H33" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="8">
-        <v>1</v>
-      </c>
-      <c r="E34" s="9">
-        <v>1</v>
-      </c>
-      <c r="F34" s="10">
-        <v>1</v>
-      </c>
-      <c r="G34" s="11">
-        <v>3</v>
-      </c>
-      <c r="H34" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="8">
-        <v>1</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="11">
-        <v>2</v>
-      </c>
-      <c r="H35" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D36" s="8">
+        <v>1</v>
+      </c>
+      <c r="E36" s="9">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
         <v>120</v>
-      </c>
-      <c r="D36" s="8">
-        <v>1</v>
-      </c>
-      <c r="E36" s="9">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="11">
-        <v>2</v>
-      </c>
-      <c r="H36" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" t="s">
-        <v>121</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="9">
         <v>1</v>
       </c>
       <c r="F37" s="6"/>
-      <c r="G37" s="11">
-        <v>1</v>
-      </c>
-      <c r="H37" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="8">
         <v>1</v>
@@ -1883,46 +2309,46 @@
       <c r="F38" s="10">
         <v>1</v>
       </c>
-      <c r="G38" s="11">
-        <v>3</v>
-      </c>
-      <c r="H38" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="8">
-        <v>1</v>
-      </c>
-      <c r="E39" s="9">
-        <v>1</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="11">
-        <v>3</v>
-      </c>
-      <c r="H39" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
-        <v>77</v>
-      </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D40" s="8">
         <v>1</v>
@@ -1931,22 +2357,22 @@
       <c r="F40" s="10">
         <v>1</v>
       </c>
-      <c r="G40" s="11">
-        <v>3</v>
-      </c>
-      <c r="H40" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>190</v>
+      </c>
+      <c r="I40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
-        <v>79</v>
-      </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D41" s="8">
         <v>1</v>
@@ -1955,79 +2381,563 @@
       <c r="F41" s="10">
         <v>1</v>
       </c>
-      <c r="G41" s="11">
-        <v>3</v>
-      </c>
-      <c r="H41" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>191</v>
+      </c>
+      <c r="I41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="2"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="11">
-        <v>3</v>
-      </c>
-      <c r="H42" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
-        <v>83</v>
-      </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="9">
         <v>1</v>
       </c>
       <c r="F43" s="6"/>
-      <c r="G43" s="11">
-        <v>1</v>
-      </c>
-      <c r="H43" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
-        <v>85</v>
-      </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="8">
         <v>1</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="6"/>
-      <c r="G44" s="11">
-        <v>1</v>
-      </c>
-      <c r="H44" s="12">
-        <v>2</v>
+      <c r="G44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" t="s">
+        <v>217</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
+        <v>214</v>
+      </c>
+      <c r="C48" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" t="s">
+        <v>215</v>
+      </c>
+      <c r="C50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" t="s">
+        <v>216</v>
+      </c>
+      <c r="C51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>231</v>
+      </c>
+      <c r="C52" t="s">
+        <v>218</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>244</v>
+      </c>
+      <c r="H52" t="s">
+        <v>245</v>
+      </c>
+      <c r="J52" s="15"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>225</v>
+      </c>
+      <c r="B53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" t="s">
+        <v>238</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
+        <v>246</v>
+      </c>
+      <c r="H53" t="s">
+        <v>247</v>
+      </c>
+      <c r="J53" s="15"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>226</v>
+      </c>
+      <c r="B54" t="s">
+        <v>233</v>
+      </c>
+      <c r="C54" t="s">
+        <v>239</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>248</v>
+      </c>
+      <c r="H54" t="s">
+        <v>249</v>
+      </c>
+      <c r="J54" s="15"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" t="s">
+        <v>240</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>250</v>
+      </c>
+      <c r="H55" t="s">
+        <v>251</v>
+      </c>
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" t="s">
+        <v>241</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>252</v>
+      </c>
+      <c r="H56" t="s">
+        <v>253</v>
+      </c>
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" t="s">
+        <v>242</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>254</v>
+      </c>
+      <c r="H57" t="s">
+        <v>324</v>
+      </c>
+      <c r="J57" s="15"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" t="s">
+        <v>243</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>255</v>
+      </c>
+      <c r="J58" s="15"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>262</v>
+      </c>
+      <c r="B59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C59" t="s">
+        <v>268</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>263</v>
+      </c>
+      <c r="B60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>264</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" t="s">
+        <v>269</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B62" t="s">
+        <v>259</v>
+      </c>
+      <c r="C62" t="s">
+        <v>271</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B63" t="s">
+        <v>260</v>
+      </c>
+      <c r="C63" t="s">
+        <v>272</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B64" t="s">
+        <v>261</v>
+      </c>
+      <c r="C64" t="s">
+        <v>273</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C65" t="s">
+        <v>287</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="G65" t="s">
+        <v>291</v>
+      </c>
+      <c r="H65" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B66" t="s">
+        <v>286</v>
+      </c>
+      <c r="C66" t="s">
+        <v>286</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="G66" t="s">
+        <v>293</v>
+      </c>
+      <c r="H66" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B67" t="s">
+        <v>274</v>
+      </c>
+      <c r="C67" t="s">
+        <v>282</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="G67" t="s">
+        <v>244</v>
+      </c>
+      <c r="H67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68" t="s">
+        <v>275</v>
+      </c>
+      <c r="C68" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="s">
+        <v>289</v>
+      </c>
+      <c r="H68" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69" t="s">
+        <v>276</v>
+      </c>
+      <c r="C69" t="s">
+        <v>283</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="G69" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2049,99 +2959,99 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
         <v>136</v>
-      </c>
-      <c r="B1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2151,31 +3061,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19893C-3433-4E5A-B231-F0E5406405D5}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -2183,10 +3093,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>303</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -2194,7 +3104,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>304</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2205,10 +3115,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>305</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -2216,51 +3126,51 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>322</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>160</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>323</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>306</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -2271,10 +3181,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>307</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -2282,13 +3192,366 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>308</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>310</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>312</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>316</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>321</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>320</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>319</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F522EADF-145D-4C25-80A5-C8FF6EE41593}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>52</v>
+      </c>
+      <c r="F5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2296,22 +3559,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8811BF-08BF-4B4B-A1A4-780FC5698012}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prof recognition fixed added M1 ISI,Resys
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFF4FC4-693D-4165-B999-B170BF567616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA388B-B2D0-44A8-9C75-842AEE1BC683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
     <sheet name="Professors" sheetId="3" r:id="rId2"/>
     <sheet name="Rooms" sheetId="4" r:id="rId3"/>
     <sheet name="Promos" sheetId="6" r:id="rId4"/>
-    <sheet name="L3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="428">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -481,12 +480,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>groups</t>
-  </si>
-  <si>
-    <t>capacity</t>
-  </si>
-  <si>
     <t>Mechaoui(*)</t>
   </si>
   <si>
@@ -550,9 +543,6 @@
     <t>prof_tp</t>
   </si>
   <si>
-    <t>BENIDRIS(7)</t>
-  </si>
-  <si>
     <t>M. Ould Ali M(2),Mme Ablaoui(2),Mme Bendehmane H(2),M. Kaid(4),Mlle FERRAOUN A.(2),Mlle Bouabdelli(2)</t>
   </si>
   <si>
@@ -565,36 +555,9 @@
     <t xml:space="preserve"> Physique 2(électricité générale)</t>
   </si>
   <si>
-    <t>MECHAOUI(7)</t>
-  </si>
-  <si>
     <t>HOCINE(7)</t>
   </si>
   <si>
-    <t>DELALI(7)</t>
-  </si>
-  <si>
-    <t>SEHABA(5),HENNI K(4)</t>
-  </si>
-  <si>
-    <t>ABID(6),BETOUATI(3)</t>
-  </si>
-  <si>
-    <t>LAREDJ(3),BOUZEBIBA(6)</t>
-  </si>
-  <si>
-    <t>BENHAMED(7), MOUSSA(2)</t>
-  </si>
-  <si>
-    <t>BESSAOUD(3),BESNASSI(3),MIDOUN(3)</t>
-  </si>
-  <si>
-    <t>KENNICHE(3),DJAHAFI(3),HENNI K(3)</t>
-  </si>
-  <si>
-    <t>MIROUD(3),BETOUATI(4),MEROUFEL(2)</t>
-  </si>
-  <si>
     <t>MECHAOUI M. D.G(1)</t>
   </si>
   <si>
@@ -610,9 +573,6 @@
     <t>MIDOUN M.(1)</t>
   </si>
   <si>
-    <t>HENNI F(1),KAID SLIMANE(3),BENSALLOUA(4),BENAMEUR(3),MOUMEN(1),Zahmani(2)</t>
-  </si>
-  <si>
     <t>HENNI F(2)</t>
   </si>
   <si>
@@ -931,12 +891,6 @@
     <t>HASSAINE(3),HAMAMI(8),DJAHAFI(3)</t>
   </si>
   <si>
-    <t>KENNICHE(3),KHIAT(2),DJAHAFI(2),BOUZEBIBA(2)</t>
-  </si>
-  <si>
-    <t>MAGHNI SANDID(5),MENAD(3),MIROUD(1)</t>
-  </si>
-  <si>
     <t>HOCINE N.(7)</t>
   </si>
   <si>
@@ -1004,6 +958,360 @@
   </si>
   <si>
     <t>Mme Bendahmane Hafida(2)</t>
+  </si>
+  <si>
+    <t>Techniques de programmation avancées</t>
+  </si>
+  <si>
+    <t>Ingénierie logicielle</t>
+  </si>
+  <si>
+    <t>Apprentissage machine</t>
+  </si>
+  <si>
+    <t>Analyse de données</t>
+  </si>
+  <si>
+    <t>Modélisation et simulation</t>
+  </si>
+  <si>
+    <t>Architecture logicielle orientée service</t>
+  </si>
+  <si>
+    <t>Sécurité des SI</t>
+  </si>
+  <si>
+    <t>Ontologie et Web Sémantique</t>
+  </si>
+  <si>
+    <t>Fouille de données</t>
+  </si>
+  <si>
+    <t>Recherche opérationnelle</t>
+  </si>
+  <si>
+    <t>Systèmes multi-agents</t>
+  </si>
+  <si>
+    <t>Diffusion de contenus numériques</t>
+  </si>
+  <si>
+    <t>Systèmes d’information décisionnels</t>
+  </si>
+  <si>
+    <t>Ingénierie dirigée par les modèles</t>
+  </si>
+  <si>
+    <t>Technologies émergentes en ISI</t>
+  </si>
+  <si>
+    <t>Réseaux avancés et grandes distances</t>
+  </si>
+  <si>
+    <t>Cryptographie</t>
+  </si>
+  <si>
+    <t>Cloud computing</t>
+  </si>
+  <si>
+    <t>Réseaux sans fil et mobiles</t>
+  </si>
+  <si>
+    <t>Gestion des services réseaux</t>
+  </si>
+  <si>
+    <t>Virtualisation des systèmes</t>
+  </si>
+  <si>
+    <t>Sécurité des réseaux et internet</t>
+  </si>
+  <si>
+    <t>Administration des serveurs de BD et applications</t>
+  </si>
+  <si>
+    <t>Programmation réseaux</t>
+  </si>
+  <si>
+    <t>Administration et Organisation des SI</t>
+  </si>
+  <si>
+    <t>Administration des serveurs Microsoft</t>
+  </si>
+  <si>
+    <t>Configuration des serveurs de messagerie</t>
+  </si>
+  <si>
+    <t>Gestion du routage</t>
+  </si>
+  <si>
+    <t>Administration de serveur Linux</t>
+  </si>
+  <si>
+    <t>Supervision des réseaux</t>
+  </si>
+  <si>
+    <t>TPA</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>BDDA</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>ModSim</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>AOSI</t>
+  </si>
+  <si>
+    <t>Bases de données avancées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administration et organisation des SI </t>
+  </si>
+  <si>
+    <t>ALOS</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>OWS</t>
+  </si>
+  <si>
+    <t>FDD</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion d’entreprise </t>
+  </si>
+  <si>
+    <t>Gestion de projets</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>DCN</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>IDM</t>
+  </si>
+  <si>
+    <t>TEISI</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Rédaction</t>
+  </si>
+  <si>
+    <t>Cloud et virtualisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction à l’entrepreneuriat </t>
+  </si>
+  <si>
+    <t>Rédaction scientifique</t>
+  </si>
+  <si>
+    <t>RAGD</t>
+  </si>
+  <si>
+    <t>CRYPTO</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>RSFM</t>
+  </si>
+  <si>
+    <t>Gestion d’entreprise</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>GSR</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>SRI</t>
+  </si>
+  <si>
+    <t>ASBDA</t>
+  </si>
+  <si>
+    <t>ASM</t>
+  </si>
+  <si>
+    <t>CSM</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>ASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche Opérationnelle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de projet </t>
+  </si>
+  <si>
+    <t>Introduction à l’entrepreneuriat</t>
+  </si>
+  <si>
+    <t>BENTAOUZA (4)</t>
+  </si>
+  <si>
+    <t>KHELIFA N.(1)</t>
+  </si>
+  <si>
+    <t>MOUSSA M.(1)</t>
+  </si>
+  <si>
+    <t>BENTAOUZA C(1)</t>
+  </si>
+  <si>
+    <t>DJEBBARA R.(1)</t>
+  </si>
+  <si>
+    <t>MOUMEN M.(1)</t>
+  </si>
+  <si>
+    <t>BAHNES N.(1)</t>
+  </si>
+  <si>
+    <t>MEROUFEL B.(1)</t>
+  </si>
+  <si>
+    <t>LAREDJ A (1)</t>
+  </si>
+  <si>
+    <t>LAREDJ (1)</t>
+  </si>
+  <si>
+    <t>FILALI (1)</t>
+  </si>
+  <si>
+    <t>BENTAOUZA  (1)</t>
+  </si>
+  <si>
+    <t>HOCINE N (1)</t>
+  </si>
+  <si>
+    <t>KHIAT(1)</t>
+  </si>
+  <si>
+    <t>LAREDJ A.(1)</t>
+  </si>
+  <si>
+    <t>FILALI F.(1)</t>
+  </si>
+  <si>
+    <t>HABIB ZAHMANI M(1)</t>
+  </si>
+  <si>
+    <t>HOCINE N(1)</t>
+  </si>
+  <si>
+    <t>KHELIFA N(1)</t>
+  </si>
+  <si>
+    <t>BAHNES N.(2) , MIROUD(2)</t>
+  </si>
+  <si>
+    <t>HENNI F(1),KAID SLIMANE(3),BENSALLOUA(4),BENAMEUR(3),MOUMEN(1),HABIB ZAHMANI M(2)</t>
+  </si>
+  <si>
+    <t>HABIB ZAHMANI M(4)</t>
+  </si>
+  <si>
+    <t>MECHAOUI M. D.G(7)</t>
+  </si>
+  <si>
+    <t>BENHAMED(7), MOUSSA M.(2)</t>
+  </si>
+  <si>
+    <t>MOUSSA M.(4)</t>
+  </si>
+  <si>
+    <t>BESSAOUD K.(3),BESNASSI(3),MIDOUN(3)</t>
+  </si>
+  <si>
+    <t>KENNICHE A.(3),KHIAT(2),DJAHAFI(2),BOUZEBIBA(2)</t>
+  </si>
+  <si>
+    <t>KENNICHE A.(3),DJAHAFI(3),HENNI K(3)</t>
+  </si>
+  <si>
+    <t>MAGHNI SANDID Z.(5),MENAD(3),MIROUD(1)</t>
+  </si>
+  <si>
+    <t>LAREDJ A. M(3),BOUZEBIBA(6)</t>
+  </si>
+  <si>
+    <t>ABID M.(6),BETOUATI(3)</t>
+  </si>
+  <si>
+    <t>SEHABA K.(5),HENNI K(4)</t>
+  </si>
+  <si>
+    <t>BENIDRIS F.Z(7)</t>
+  </si>
+  <si>
+    <t>DELALI A.(7)</t>
+  </si>
+  <si>
+    <t>DJEBBARA R.(4)</t>
+  </si>
+  <si>
+    <t>MEROUFEL B.(4)</t>
+  </si>
+  <si>
+    <t>MIROUD(3),BETOUATI(4),MEROUFEL B.(2)</t>
+  </si>
+  <si>
+    <t>KHELIFA N.(2) ,KHIAT (2)</t>
+  </si>
+  <si>
+    <t>KHELIFA N.(2) ,KHIAT(2)</t>
+  </si>
+  <si>
+    <t>M1-ISI</t>
+  </si>
+  <si>
+    <t>M1-RéSys</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1146,6 +1454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1460,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA34FF-0E82-47CA-8C99-448458D5C5EE}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView topLeftCell="C45" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="C88" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,13 +1806,13 @@
         <v>132</v>
       </c>
       <c r="G1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
         <v>170</v>
-      </c>
-      <c r="H1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1662,10 +1971,10 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="H9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1686,10 +1995,10 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1712,13 +2021,13 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H11" t="s">
-        <v>193</v>
+        <v>407</v>
       </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1739,10 +2048,10 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="H12" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1763,10 +2072,10 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="H13" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1785,7 +2094,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1806,10 +2115,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H15" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1817,7 +2126,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C16" t="s">
         <v>90</v>
@@ -1830,10 +2139,10 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="H16" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2000,13 +2309,13 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="H24" t="s">
-        <v>185</v>
+        <v>412</v>
       </c>
       <c r="I24" t="s">
-        <v>185</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2029,13 +2338,13 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="H25" t="s">
-        <v>300</v>
+        <v>413</v>
       </c>
       <c r="I25" t="s">
-        <v>186</v>
+        <v>414</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2058,13 +2367,13 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H26" t="s">
-        <v>301</v>
+        <v>415</v>
       </c>
       <c r="I26" t="s">
-        <v>187</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2087,13 +2396,13 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="H27" t="s">
-        <v>183</v>
+        <v>416</v>
       </c>
       <c r="I27" t="s">
-        <v>184</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2114,10 +2423,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>417</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2138,10 +2447,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="I29" t="s">
-        <v>181</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2310,10 +2619,10 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I38" t="s">
-        <v>178</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2334,10 +2643,10 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="H39" t="s">
-        <v>173</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2358,10 +2667,10 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="I40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2382,10 +2691,10 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="I41" t="s">
-        <v>180</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2418,7 +2727,7 @@
       </c>
       <c r="F43" s="6"/>
       <c r="H43" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2437,18 +2746,18 @@
       <c r="E44" s="2"/>
       <c r="F44" s="6"/>
       <c r="G44" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C45" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -2462,10 +2771,10 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C46" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -2476,13 +2785,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B47" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C47" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2496,10 +2805,10 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C48" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2530,13 +2839,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B50" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2544,13 +2853,13 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2558,13 +2867,13 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B52" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C52" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2573,23 +2882,23 @@
         <v>2</v>
       </c>
       <c r="G52" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="H52" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" t="s">
         <v>225</v>
       </c>
-      <c r="B53" t="s">
-        <v>232</v>
-      </c>
-      <c r="C53" t="s">
-        <v>238</v>
-      </c>
       <c r="D53">
         <v>1</v>
       </c>
@@ -2597,22 +2906,22 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="H53" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" t="s">
         <v>226</v>
-      </c>
-      <c r="B54" t="s">
-        <v>233</v>
-      </c>
-      <c r="C54" t="s">
-        <v>239</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2621,23 +2930,23 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="H54" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>214</v>
+      </c>
+      <c r="B55" t="s">
+        <v>221</v>
+      </c>
+      <c r="C55" t="s">
         <v>227</v>
       </c>
-      <c r="B55" t="s">
-        <v>234</v>
-      </c>
-      <c r="C55" t="s">
-        <v>240</v>
-      </c>
       <c r="D55">
         <v>1</v>
       </c>
@@ -2648,23 +2957,23 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="H55" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" t="s">
         <v>228</v>
       </c>
-      <c r="B56" t="s">
-        <v>235</v>
-      </c>
-      <c r="C56" t="s">
-        <v>241</v>
-      </c>
       <c r="D56">
         <v>1</v>
       </c>
@@ -2672,23 +2981,23 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="H56" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" t="s">
+        <v>223</v>
+      </c>
+      <c r="C57" t="s">
         <v>229</v>
       </c>
-      <c r="B57" t="s">
-        <v>236</v>
-      </c>
-      <c r="C57" t="s">
-        <v>242</v>
-      </c>
       <c r="D57">
         <v>1</v>
       </c>
@@ -2696,23 +3005,23 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="H57" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" t="s">
+        <v>224</v>
+      </c>
+      <c r="C58" t="s">
         <v>230</v>
       </c>
-      <c r="B58" t="s">
-        <v>237</v>
-      </c>
-      <c r="C58" t="s">
-        <v>243</v>
-      </c>
       <c r="D58">
         <v>1</v>
       </c>
@@ -2720,19 +3029,19 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B59" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C59" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -2743,13 +3052,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="B60" t="s">
+        <v>244</v>
+      </c>
+      <c r="C60" t="s">
         <v>257</v>
-      </c>
-      <c r="C60" t="s">
-        <v>270</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2760,13 +3069,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B61" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C61" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2777,13 +3086,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C62" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2794,13 +3103,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C63" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2814,27 +3123,27 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B64" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C64" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C65" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -2843,21 +3152,21 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="H65" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B66" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="C66" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -2866,21 +3175,21 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="H66" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B67" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="C67" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -2889,21 +3198,21 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="H67" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B68" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C68" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -2912,27 +3221,807 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="H68" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="B69" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C69" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>292</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>310</v>
+      </c>
+      <c r="C70" t="s">
+        <v>340</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>311</v>
+      </c>
+      <c r="C71" t="s">
+        <v>341</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>349</v>
+      </c>
+      <c r="C72" t="s">
+        <v>343</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>312</v>
+      </c>
+      <c r="C73" t="s">
+        <v>344</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>313</v>
+      </c>
+      <c r="C74" t="s">
+        <v>342</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>314</v>
+      </c>
+      <c r="C75" t="s">
+        <v>346</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>356</v>
+      </c>
+      <c r="C76" t="s">
+        <v>347</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>350</v>
+      </c>
+      <c r="C77" t="s">
+        <v>348</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>388</v>
+      </c>
+      <c r="H77" t="s">
+        <v>424</v>
+      </c>
+      <c r="I77" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>315</v>
+      </c>
+      <c r="C78" t="s">
+        <v>351</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78" t="s">
+        <v>389</v>
+      </c>
+      <c r="I78" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>316</v>
+      </c>
+      <c r="C79" t="s">
+        <v>352</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>390</v>
+      </c>
+      <c r="I79" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>317</v>
+      </c>
+      <c r="C80" t="s">
+        <v>353</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80" t="s">
+        <v>391</v>
+      </c>
+      <c r="I80" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>318</v>
+      </c>
+      <c r="C81" t="s">
+        <v>354</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="s">
+        <v>392</v>
+      </c>
+      <c r="I81" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>319</v>
+      </c>
+      <c r="C82" t="s">
+        <v>345</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82" t="s">
+        <v>393</v>
+      </c>
+      <c r="H82" t="s">
+        <v>406</v>
+      </c>
+      <c r="I82" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>357</v>
+      </c>
+      <c r="C83" t="s">
+        <v>355</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>320</v>
+      </c>
+      <c r="C84" t="s">
+        <v>358</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84" t="s">
+        <v>394</v>
+      </c>
+      <c r="I84" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>321</v>
+      </c>
+      <c r="C85" t="s">
+        <v>359</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>322</v>
+      </c>
+      <c r="C86" t="s">
+        <v>360</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>323</v>
+      </c>
+      <c r="C87" t="s">
+        <v>361</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>324</v>
+      </c>
+      <c r="C88" t="s">
+        <v>362</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>366</v>
+      </c>
+      <c r="C89" t="s">
+        <v>363</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>367</v>
+      </c>
+      <c r="C90" t="s">
+        <v>364</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>368</v>
+      </c>
+      <c r="C91" t="s">
+        <v>365</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>325</v>
+      </c>
+      <c r="C92" t="s">
+        <v>369</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>326</v>
+      </c>
+      <c r="C93" t="s">
+        <v>370</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>327</v>
+      </c>
+      <c r="C94" t="s">
+        <v>371</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>328</v>
+      </c>
+      <c r="C95" t="s">
+        <v>372</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>349</v>
+      </c>
+      <c r="C96" t="s">
+        <v>343</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>373</v>
+      </c>
+      <c r="C97" t="s">
+        <v>347</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>329</v>
+      </c>
+      <c r="C98" t="s">
+        <v>375</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" t="s">
+        <v>401</v>
+      </c>
+      <c r="H98" t="s">
+        <v>395</v>
+      </c>
+      <c r="I98" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>330</v>
+      </c>
+      <c r="C99" t="s">
+        <v>376</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" t="s">
+        <v>402</v>
+      </c>
+      <c r="I99" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>331</v>
+      </c>
+      <c r="C100" t="s">
+        <v>378</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" t="s">
+        <v>390</v>
+      </c>
+      <c r="I100" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>332</v>
+      </c>
+      <c r="C101" t="s">
+        <v>379</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="G101" t="s">
+        <v>403</v>
+      </c>
+      <c r="I101" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>333</v>
+      </c>
+      <c r="C102" t="s">
+        <v>374</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>404</v>
+      </c>
+      <c r="I102" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>334</v>
+      </c>
+      <c r="C103" t="s">
+        <v>348</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>405</v>
+      </c>
+      <c r="H103" t="s">
+        <v>400</v>
+      </c>
+      <c r="I103" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>384</v>
+      </c>
+      <c r="C104" t="s">
+        <v>345</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>393</v>
+      </c>
+      <c r="H104" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>385</v>
+      </c>
+      <c r="C105" t="s">
+        <v>355</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="G105" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>335</v>
+      </c>
+      <c r="C106" t="s">
+        <v>380</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>336</v>
+      </c>
+      <c r="C107" t="s">
+        <v>381</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>337</v>
+      </c>
+      <c r="C108" t="s">
+        <v>382</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>338</v>
+      </c>
+      <c r="C109" t="s">
+        <v>383</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>339</v>
+      </c>
+      <c r="C110" t="s">
+        <v>377</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>386</v>
+      </c>
+      <c r="C111" t="s">
+        <v>364</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2976,13 +4065,13 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2990,13 +4079,13 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3004,13 +4093,13 @@
         <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,10 +4107,10 @@
         <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3029,10 +4118,10 @@
         <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,10 +4129,10 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3051,7 +4140,7 @@
         <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3063,8 +4152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19893C-3433-4E5A-B231-F0E5406405D5}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,10 +4171,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>304</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -3093,10 +4182,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -3104,10 +4193,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -3115,10 +4204,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -3126,51 +4215,51 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>230</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>230</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>230</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>360</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -3181,7 +4270,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>307</v>
+        <v>144</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -3192,7 +4281,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>308</v>
+        <v>140</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3203,7 +4292,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -3214,10 +4303,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>143</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>25</v>
@@ -3225,10 +4314,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>142</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -3236,10 +4325,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>141</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>25</v>
@@ -3247,7 +4336,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -3258,10 +4347,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>297</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>25</v>
@@ -3269,10 +4358,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>296</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>25</v>
@@ -3280,10 +4369,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>25</v>
@@ -3291,7 +4380,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -3302,7 +4391,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>293</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -3313,7 +4402,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>292</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3324,7 +4413,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3335,54 +4424,54 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>45</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>25</v>
@@ -3390,10 +4479,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>25</v>
@@ -3401,10 +4490,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>25</v>
@@ -3412,10 +4501,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>319</v>
+        <v>149</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>25</v>
@@ -3423,7 +4512,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
-    <sortCondition ref="A2:A32"/>
+    <sortCondition descending="1" ref="A2:A32"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3432,31 +4521,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F522EADF-145D-4C25-80A5-C8FF6EE41593}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" t="s">
         <v>161</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -3476,7 +4565,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3496,7 +4585,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3516,7 +4605,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3536,7 +4625,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3552,89 +4641,49 @@
       </c>
       <c r="F6">
         <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>77</v>
+      </c>
+      <c r="F7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
+      <c r="F8">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8811BF-08BF-4B4B-A1A4-780FC5698012}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sized time slots in exports
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA388B-B2D0-44A8-9C75-842AEE1BC683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3CD2A-162B-484A-8653-4B0B70DD20FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="420">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -579,9 +579,6 @@
     <t>HASSAINE(2)</t>
   </si>
   <si>
-    <t>HENNI K. (2)</t>
-  </si>
-  <si>
     <t>BESSAOUD K.(1)</t>
   </si>
   <si>
@@ -1191,9 +1188,6 @@
     <t>Introduction à l’entrepreneuriat</t>
   </si>
   <si>
-    <t>BENTAOUZA (4)</t>
-  </si>
-  <si>
     <t>KHELIFA N.(1)</t>
   </si>
   <si>
@@ -1215,21 +1209,6 @@
     <t>MEROUFEL B.(1)</t>
   </si>
   <si>
-    <t>LAREDJ A (1)</t>
-  </si>
-  <si>
-    <t>LAREDJ (1)</t>
-  </si>
-  <si>
-    <t>FILALI (1)</t>
-  </si>
-  <si>
-    <t>BENTAOUZA  (1)</t>
-  </si>
-  <si>
-    <t>HOCINE N (1)</t>
-  </si>
-  <si>
     <t>KHIAT(1)</t>
   </si>
   <si>
@@ -1242,12 +1221,6 @@
     <t>HABIB ZAHMANI M(1)</t>
   </si>
   <si>
-    <t>HOCINE N(1)</t>
-  </si>
-  <si>
-    <t>KHELIFA N(1)</t>
-  </si>
-  <si>
     <t>BAHNES N.(2) , MIROUD(2)</t>
   </si>
   <si>
@@ -1266,9 +1239,6 @@
     <t>MOUSSA M.(4)</t>
   </si>
   <si>
-    <t>BESSAOUD K.(3),BESNASSI(3),MIDOUN(3)</t>
-  </si>
-  <si>
     <t>KENNICHE A.(3),KHIAT(2),DJAHAFI(2),BOUZEBIBA(2)</t>
   </si>
   <si>
@@ -1302,9 +1272,6 @@
     <t>MIROUD(3),BETOUATI(4),MEROUFEL B.(2)</t>
   </si>
   <si>
-    <t>KHELIFA N.(2) ,KHIAT (2)</t>
-  </si>
-  <si>
     <t>KHELIFA N.(2) ,KHIAT(2)</t>
   </si>
   <si>
@@ -1312,6 +1279,15 @@
   </si>
   <si>
     <t>M1-RéSys</t>
+  </si>
+  <si>
+    <t>HENNI K.(2)</t>
+  </si>
+  <si>
+    <t>BENTAOUZA C(4)</t>
+  </si>
+  <si>
+    <t>BESSAOUD K.(3),BESNASSI(3),MIDOUN M.(3)</t>
   </si>
 </sst>
 </file>
@@ -1771,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA34FF-0E82-47CA-8C99-448458D5C5EE}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C88" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1947,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H9" t="s">
         <v>171</v>
@@ -2024,10 +2000,10 @@
         <v>181</v>
       </c>
       <c r="H11" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="I11" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2051,7 +2027,7 @@
         <v>182</v>
       </c>
       <c r="H12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2072,10 +2048,10 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" t="s">
+        <v>189</v>
+      </c>
+      <c r="H13" t="s">
         <v>190</v>
-      </c>
-      <c r="H13" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2094,7 +2070,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
       <c r="G14" t="s">
-        <v>183</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2115,10 +2091,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
+        <v>191</v>
+      </c>
+      <c r="H15" t="s">
         <v>192</v>
-      </c>
-      <c r="H15" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2139,10 +2115,10 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" t="s">
+        <v>283</v>
+      </c>
+      <c r="H16" t="s">
         <v>284</v>
-      </c>
-      <c r="H16" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2309,13 +2285,13 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H24" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="I24" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2338,13 +2314,13 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H25" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="I25" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2367,13 +2343,13 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H26" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="I26" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2396,13 +2372,13 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H27" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="I27" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2423,10 +2399,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2447,10 +2423,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I29" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2622,7 +2598,7 @@
         <v>176</v>
       </c>
       <c r="I38" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2646,7 +2622,7 @@
         <v>177</v>
       </c>
       <c r="H39" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2694,7 +2670,7 @@
         <v>179</v>
       </c>
       <c r="I41" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2727,7 +2703,7 @@
       </c>
       <c r="F43" s="6"/>
       <c r="H43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2751,13 +2727,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" t="s">
         <v>194</v>
       </c>
-      <c r="B45" t="s">
-        <v>195</v>
-      </c>
       <c r="C45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -2771,10 +2747,10 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -2785,13 +2761,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2805,10 +2781,10 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2839,13 +2815,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2853,13 +2829,13 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2867,13 +2843,13 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2882,22 +2858,22 @@
         <v>2</v>
       </c>
       <c r="G52" t="s">
+        <v>230</v>
+      </c>
+      <c r="H52" t="s">
         <v>231</v>
-      </c>
-      <c r="H52" t="s">
-        <v>232</v>
       </c>
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2906,22 +2882,22 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
+        <v>232</v>
+      </c>
+      <c r="H53" t="s">
         <v>233</v>
-      </c>
-      <c r="H53" t="s">
-        <v>234</v>
       </c>
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2930,22 +2906,22 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
+        <v>234</v>
+      </c>
+      <c r="H54" t="s">
         <v>235</v>
-      </c>
-      <c r="H54" t="s">
-        <v>236</v>
       </c>
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2957,22 +2933,22 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
+        <v>236</v>
+      </c>
+      <c r="H55" t="s">
         <v>237</v>
-      </c>
-      <c r="H55" t="s">
-        <v>238</v>
       </c>
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2981,22 +2957,22 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
+        <v>238</v>
+      </c>
+      <c r="H56" t="s">
         <v>239</v>
-      </c>
-      <c r="H56" t="s">
-        <v>240</v>
       </c>
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3005,22 +2981,22 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3029,19 +3005,19 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -3052,13 +3028,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -3069,13 +3045,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3086,13 +3062,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C62" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3103,13 +3079,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -3123,13 +3099,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B64" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3137,13 +3113,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3152,21 +3128,21 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H65" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -3175,21 +3151,21 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
+        <v>279</v>
+      </c>
+      <c r="H66" t="s">
         <v>280</v>
-      </c>
-      <c r="H66" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B67" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C67" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -3198,21 +3174,21 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H67" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -3221,35 +3197,35 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
+        <v>275</v>
+      </c>
+      <c r="H68" t="s">
         <v>276</v>
-      </c>
-      <c r="H68" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C70" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -3263,10 +3239,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C71" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -3280,10 +3256,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C72" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -3297,10 +3273,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C73" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3314,10 +3290,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C74" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -3331,10 +3307,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C75" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -3348,10 +3324,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3365,10 +3341,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C77" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -3380,21 +3356,21 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H77" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="I77" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C78" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3406,18 +3382,18 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I78" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C79" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -3429,18 +3405,18 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I79" t="s">
-        <v>387</v>
+        <v>418</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C80" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3452,18 +3428,18 @@
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I80" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C81" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -3475,18 +3451,18 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I81" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C82" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -3498,21 +3474,21 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H82" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="I82" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C83" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3529,10 +3505,10 @@
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C84" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -3544,18 +3520,18 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I84" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -3569,10 +3545,10 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C86" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3586,10 +3562,10 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C87" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -3603,10 +3579,10 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C88" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -3620,10 +3596,10 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C89" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3637,10 +3613,10 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C90" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -3654,10 +3630,10 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C91" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -3671,10 +3647,10 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C92" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -3688,10 +3664,10 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C93" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -3705,10 +3681,10 @@
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C94" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -3719,10 +3695,10 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C95" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -3736,10 +3712,10 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C96" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -3750,10 +3726,10 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C97" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -3761,10 +3737,10 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C98" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -3776,21 +3752,21 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="H98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I98" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C99" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -3799,18 +3775,18 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I99" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C100" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -3819,35 +3795,35 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I100" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C101" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="I101" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C102" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -3856,18 +3832,18 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>404</v>
+        <v>178</v>
       </c>
       <c r="I102" t="s">
-        <v>399</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C103" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -3879,21 +3855,21 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="H103" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="I103" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C104" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -3902,18 +3878,18 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H104" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C105" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -3924,10 +3900,10 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C106" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -3941,10 +3917,10 @@
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C107" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -3958,10 +3934,10 @@
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C108" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3975,10 +3951,10 @@
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C109" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -3992,10 +3968,10 @@
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C110" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -4009,10 +3985,10 @@
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C111" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -4171,7 +4147,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -4182,7 +4158,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4193,7 +4169,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -4204,7 +4180,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -4215,7 +4191,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4226,7 +4202,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -4259,7 +4235,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -4292,7 +4268,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -4336,7 +4312,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -4347,7 +4323,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -4358,7 +4334,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -4369,7 +4345,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -4380,7 +4356,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -4391,7 +4367,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -4402,7 +4378,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -4413,7 +4389,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -4446,7 +4422,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4457,7 +4433,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4468,7 +4444,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -4479,7 +4455,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -4490,7 +4466,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -4645,7 +4621,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4665,7 +4641,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="B8">
         <v>1</v>

</xml_diff>

<commit_message>
added M1 AF,M1 MCO and run time analytics
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3CD2A-162B-484A-8653-4B0B70DD20FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDD439C-1649-4EF6-A3C2-3E9E94E57AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="464">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -543,9 +543,6 @@
     <t>prof_tp</t>
   </si>
   <si>
-    <t>M. Ould Ali M(2),Mme Ablaoui(2),Mme Bendehmane H(2),M. Kaid(4),Mlle FERRAOUN A.(2),Mlle Bouabdelli(2)</t>
-  </si>
-  <si>
     <t>M. Medeghri Ahmed(2)</t>
   </si>
   <si>
@@ -852,9 +849,6 @@
     <t>TOL</t>
   </si>
   <si>
-    <t>M. Andasmas(2)</t>
-  </si>
-  <si>
     <t>M. BELARBI Lakehal(1)</t>
   </si>
   <si>
@@ -1288,6 +1282,144 @@
   </si>
   <si>
     <t>BESSAOUD K.(3),BESNASSI(3),MIDOUN M.(3)</t>
+  </si>
+  <si>
+    <t>M1-AF</t>
+  </si>
+  <si>
+    <t>M1-MCO</t>
+  </si>
+  <si>
+    <t>Analyse Complexe II</t>
+  </si>
+  <si>
+    <t>M. BELAIDI Benharrat(1)</t>
+  </si>
+  <si>
+    <t>Th. Des Opérateurs II</t>
+  </si>
+  <si>
+    <t>M. B. BENDOUKHA(1)</t>
+  </si>
+  <si>
+    <t>Géo. Diff II</t>
+  </si>
+  <si>
+    <t>Distributions II</t>
+  </si>
+  <si>
+    <t>M. BOUZIT Hamid(1)</t>
+  </si>
+  <si>
+    <t>EDP II</t>
+  </si>
+  <si>
+    <t>M. Andasmas M(1)</t>
+  </si>
+  <si>
+    <t>Statistiques II</t>
+  </si>
+  <si>
+    <t>Mlle Dj.BENSIKADDOUR(1)</t>
+  </si>
+  <si>
+    <t>Semi-Groupes</t>
+  </si>
+  <si>
+    <t>Mlle Medeghri Ahmed(1)</t>
+  </si>
+  <si>
+    <t>Anglais II</t>
+  </si>
+  <si>
+    <t>M. Dahmani Z.(1)</t>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t>TO2</t>
+  </si>
+  <si>
+    <t>Dis2</t>
+  </si>
+  <si>
+    <t>EDP2</t>
+  </si>
+  <si>
+    <t>GéoDiff2</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>STAT2</t>
+  </si>
+  <si>
+    <t>SEMIGROUP</t>
+  </si>
+  <si>
+    <t>Anglais2</t>
+  </si>
+  <si>
+    <t>Modélisation 2</t>
+  </si>
+  <si>
+    <t>Mod2</t>
+  </si>
+  <si>
+    <t>Mlle Bouzid Leila(1)</t>
+  </si>
+  <si>
+    <t>OAF 2</t>
+  </si>
+  <si>
+    <t>Mr S. M. Bahri(1)</t>
+  </si>
+  <si>
+    <t>Th. Contrôle</t>
+  </si>
+  <si>
+    <t>TCONTROL</t>
+  </si>
+  <si>
+    <t>Mr. BOUAGADA(1)</t>
+  </si>
+  <si>
+    <t>Cal. Fract 1</t>
+  </si>
+  <si>
+    <t>CFRAC</t>
+  </si>
+  <si>
+    <t>M. Zoubir DAHMANI(1)</t>
+  </si>
+  <si>
+    <t>Th. Des Graphes</t>
+  </si>
+  <si>
+    <t>Mr Ablaoui H.(1)</t>
+  </si>
+  <si>
+    <t>Prog. Quadratique</t>
+  </si>
+  <si>
+    <t>PROGQUAD</t>
+  </si>
+  <si>
+    <t>M. AMIR A.(1)</t>
+  </si>
+  <si>
+    <t>Latex</t>
+  </si>
+  <si>
+    <t>Mme Bouabdelli(1)</t>
+  </si>
+  <si>
+    <t>M. Ould Ali M(2),Mme Ablaoui(2),Mme Bendehmane H(2),M. Kaid(4),Mlle FERRAOUN A.(2),Mme Bouabdelli(2)</t>
+  </si>
+  <si>
+    <t>M. Andasmas M(2)</t>
   </si>
 </sst>
 </file>
@@ -1745,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA34FF-0E82-47CA-8C99-448458D5C5EE}">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,10 +2079,10 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>171</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1971,10 +2103,10 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" t="s">
+        <v>171</v>
+      </c>
+      <c r="H10" t="s">
         <v>172</v>
-      </c>
-      <c r="H10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1997,13 +2129,13 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2024,10 +2156,10 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2048,10 +2180,10 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" t="s">
+        <v>188</v>
+      </c>
+      <c r="H13" t="s">
         <v>189</v>
-      </c>
-      <c r="H13" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2070,7 +2202,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
       <c r="G14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2091,10 +2223,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
+        <v>190</v>
+      </c>
+      <c r="I15" t="s">
         <v>191</v>
-      </c>
-      <c r="H15" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2102,7 +2234,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
         <v>90</v>
@@ -2115,10 +2247,10 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2285,13 +2417,13 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2314,13 +2446,13 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H25" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I25" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2343,13 +2475,13 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H26" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2372,13 +2504,13 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2399,10 +2531,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2423,10 +2555,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I29" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2595,10 +2727,10 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I38" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2619,10 +2751,10 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H39" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2643,10 +2775,10 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2667,10 +2799,10 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I41" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2703,7 +2835,7 @@
       </c>
       <c r="F43" s="6"/>
       <c r="H43" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2722,18 +2854,18 @@
       <c r="E44" s="2"/>
       <c r="F44" s="6"/>
       <c r="G44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" t="s">
         <v>193</v>
       </c>
-      <c r="B45" t="s">
-        <v>194</v>
-      </c>
       <c r="C45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -2747,10 +2879,10 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -2761,13 +2893,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2781,10 +2913,10 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2815,13 +2947,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2829,13 +2961,13 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2843,13 +2975,13 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2858,22 +2990,22 @@
         <v>2</v>
       </c>
       <c r="G52" t="s">
+        <v>229</v>
+      </c>
+      <c r="H52" t="s">
         <v>230</v>
-      </c>
-      <c r="H52" t="s">
-        <v>231</v>
       </c>
       <c r="J52" s="15"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2882,22 +3014,22 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
+        <v>231</v>
+      </c>
+      <c r="H53" t="s">
         <v>232</v>
-      </c>
-      <c r="H53" t="s">
-        <v>233</v>
       </c>
       <c r="J53" s="15"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2906,22 +3038,22 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
+        <v>233</v>
+      </c>
+      <c r="H54" t="s">
         <v>234</v>
-      </c>
-      <c r="H54" t="s">
-        <v>235</v>
       </c>
       <c r="J54" s="15"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2933,22 +3065,22 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
+        <v>235</v>
+      </c>
+      <c r="H55" t="s">
         <v>236</v>
-      </c>
-      <c r="H55" t="s">
-        <v>237</v>
       </c>
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2957,22 +3089,22 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
+        <v>237</v>
+      </c>
+      <c r="H56" t="s">
         <v>238</v>
-      </c>
-      <c r="H56" t="s">
-        <v>239</v>
       </c>
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2981,22 +3113,22 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H57" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3005,19 +3137,19 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J58" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -3028,13 +3160,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B60" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -3045,13 +3177,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B61" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3062,13 +3194,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3079,13 +3211,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -3099,13 +3231,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3113,13 +3245,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C65" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3128,21 +3260,21 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H65" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B66" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -3151,21 +3283,21 @@
         <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H66" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B67" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C67" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -3174,21 +3306,21 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H67" t="s">
-        <v>274</v>
+        <v>463</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -3197,35 +3329,35 @@
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H68" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B69" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C69" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C70" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -3239,10 +3371,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C71" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -3256,10 +3388,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C72" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -3273,10 +3405,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C73" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3290,10 +3422,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C74" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -3307,10 +3439,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C75" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -3324,10 +3456,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C76" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3341,10 +3473,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C77" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -3356,21 +3488,21 @@
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H77" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I77" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C78" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3382,18 +3514,18 @@
         <v>1</v>
       </c>
       <c r="G78" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I78" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C79" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -3405,18 +3537,18 @@
         <v>1</v>
       </c>
       <c r="G79" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I79" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C80" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3428,18 +3560,18 @@
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I80" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C81" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -3451,18 +3583,18 @@
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I81" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C82" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -3474,21 +3606,21 @@
         <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H82" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I82" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C83" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3500,15 +3632,15 @@
         <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C84" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -3520,18 +3652,18 @@
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I84" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C85" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -3545,10 +3677,10 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C86" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3562,10 +3694,10 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C87" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -3579,10 +3711,10 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C88" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -3596,10 +3728,10 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C89" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3613,10 +3745,10 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C90" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -3630,10 +3762,10 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C91" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -3647,10 +3779,10 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C92" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -3664,10 +3796,10 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C93" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -3681,10 +3813,10 @@
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C94" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -3695,10 +3827,10 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C95" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -3712,10 +3844,10 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C96" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -3726,10 +3858,10 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C97" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -3737,10 +3869,10 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C98" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -3752,21 +3884,21 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H98" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I98" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C99" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -3775,18 +3907,18 @@
         <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I99" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C100" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -3795,35 +3927,35 @@
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I100" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C101" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I101" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C102" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -3832,18 +3964,18 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C103" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -3855,21 +3987,21 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H103" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I103" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C104" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -3878,32 +4010,32 @@
         <v>1</v>
       </c>
       <c r="G104" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H104" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C105" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D105">
         <v>1</v>
       </c>
       <c r="G105" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C106" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -3917,10 +4049,10 @@
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C107" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -3934,10 +4066,10 @@
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C108" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3951,10 +4083,10 @@
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C109" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -3968,10 +4100,10 @@
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C110" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -3985,10 +4117,10 @@
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C111" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3998,6 +4130,320 @@
       </c>
       <c r="F111">
         <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>420</v>
+      </c>
+      <c r="C112" t="s">
+        <v>435</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="G112" t="s">
+        <v>421</v>
+      </c>
+      <c r="H112" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>422</v>
+      </c>
+      <c r="C113" t="s">
+        <v>436</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="G113" t="s">
+        <v>423</v>
+      </c>
+      <c r="H113" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>424</v>
+      </c>
+      <c r="C114" t="s">
+        <v>439</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>2</v>
+      </c>
+      <c r="G114" t="s">
+        <v>273</v>
+      </c>
+      <c r="H114" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>425</v>
+      </c>
+      <c r="C115" t="s">
+        <v>437</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="G115" t="s">
+        <v>426</v>
+      </c>
+      <c r="H115" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>427</v>
+      </c>
+      <c r="C116" t="s">
+        <v>438</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>2</v>
+      </c>
+      <c r="G116" t="s">
+        <v>428</v>
+      </c>
+      <c r="H116" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>429</v>
+      </c>
+      <c r="C117" t="s">
+        <v>441</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="G117" t="s">
+        <v>430</v>
+      </c>
+      <c r="H117" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>431</v>
+      </c>
+      <c r="C118" t="s">
+        <v>442</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="G118" t="s">
+        <v>432</v>
+      </c>
+      <c r="H118" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>433</v>
+      </c>
+      <c r="C119" t="s">
+        <v>443</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="G119" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>444</v>
+      </c>
+      <c r="C120" t="s">
+        <v>445</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="G120" t="s">
+        <v>446</v>
+      </c>
+      <c r="H120" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>447</v>
+      </c>
+      <c r="C121" t="s">
+        <v>447</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="G121" t="s">
+        <v>448</v>
+      </c>
+      <c r="H121" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>449</v>
+      </c>
+      <c r="C122" t="s">
+        <v>450</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="G122" t="s">
+        <v>451</v>
+      </c>
+      <c r="H122" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>452</v>
+      </c>
+      <c r="C123" t="s">
+        <v>453</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="G123" t="s">
+        <v>454</v>
+      </c>
+      <c r="H123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>455</v>
+      </c>
+      <c r="C124" t="s">
+        <v>103</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124" t="s">
+        <v>456</v>
+      </c>
+      <c r="H124" t="s">
+        <v>456</v>
+      </c>
+      <c r="I124" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>457</v>
+      </c>
+      <c r="C125" t="s">
+        <v>458</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="G125" t="s">
+        <v>459</v>
+      </c>
+      <c r="H125" t="s">
+        <v>459</v>
+      </c>
+      <c r="I125" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>460</v>
+      </c>
+      <c r="C126" t="s">
+        <v>460</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="G126" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>440</v>
+      </c>
+      <c r="C127" t="s">
+        <v>440</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="G127" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -4147,7 +4593,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -4158,7 +4604,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4169,7 +4615,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -4180,7 +4626,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -4191,7 +4637,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4202,7 +4648,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -4235,7 +4681,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -4268,7 +4714,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -4312,7 +4758,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -4323,7 +4769,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -4334,7 +4780,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -4345,7 +4791,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -4356,7 +4802,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -4367,7 +4813,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -4378,7 +4824,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -4389,7 +4835,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -4422,7 +4868,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4433,7 +4879,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4444,7 +4890,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -4455,7 +4901,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -4466,7 +4912,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -4497,10 +4943,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F522EADF-145D-4C25-80A5-C8FF6EE41593}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4621,7 +5067,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4641,7 +5087,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4657,6 +5103,46 @@
       </c>
       <c r="F8">
         <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>112</v>
+      </c>
+      <c r="F9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>419</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>120</v>
+      </c>
+      <c r="F10">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code refactoring and typehints
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDD439C-1649-4EF6-A3C2-3E9E94E57AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82D0977-9B61-48EF-B1C8-854D38E957A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:J127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
shared resources (data shows) implemented
</commit_message>
<xml_diff>
--- a/test/Resources.xlsx
+++ b/test/Resources.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\PycharmProjects\FSEI-M_TimeTabler\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF35EF20-7897-48CF-B2D3-8D8149572770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271879AF-22AE-4FF8-A45F-50541258BAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="4950" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3BF5675C-6691-4A04-BEDC-EBF739DFC69B}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
     <sheet name="Rooms" sheetId="4" r:id="rId2"/>
     <sheet name="Promos" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="removed" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="566">
   <si>
     <t xml:space="preserve">UEF111 </t>
   </si>
@@ -1684,6 +1684,48 @@
   </si>
   <si>
     <t>S11</t>
+  </si>
+  <si>
+    <t>Physique des semiconducteurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physique statistique II  </t>
+  </si>
+  <si>
+    <t>Spectroscopie atomique et moléculaire</t>
+  </si>
+  <si>
+    <t>Méthodes numériques de simulation</t>
+  </si>
+  <si>
+    <t>PhysSemiC</t>
+  </si>
+  <si>
+    <t>PhysicStat2</t>
+  </si>
+  <si>
+    <t>MNS</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>Bencherif(1)</t>
+  </si>
+  <si>
+    <t>Benotsmane(1)</t>
+  </si>
+  <si>
+    <t>Belhouari(1)</t>
+  </si>
+  <si>
+    <t>Terki(1)</t>
+  </si>
+  <si>
+    <t>Hentit N(1)</t>
+  </si>
+  <si>
+    <t>M1-PM</t>
   </si>
 </sst>
 </file>
@@ -2141,10 +2183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA34FF-0E82-47CA-8C99-448458D5C5EE}">
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView topLeftCell="B124" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5248,6 +5290,100 @@
         <v>527</v>
       </c>
     </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>552</v>
+      </c>
+      <c r="C155" t="s">
+        <v>556</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="G155" t="s">
+        <v>560</v>
+      </c>
+      <c r="H155" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>553</v>
+      </c>
+      <c r="C156" t="s">
+        <v>557</v>
+      </c>
+      <c r="D156" s="17">
+        <v>2</v>
+      </c>
+      <c r="E156" s="17">
+        <v>1</v>
+      </c>
+      <c r="G156" t="s">
+        <v>561</v>
+      </c>
+      <c r="H156" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B157" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="C157" t="s">
+        <v>558</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="G157" t="s">
+        <v>562</v>
+      </c>
+      <c r="H157" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>554</v>
+      </c>
+      <c r="C158" t="s">
+        <v>559</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="G158" t="s">
+        <v>563</v>
+      </c>
+      <c r="H158" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>427</v>
+      </c>
+      <c r="C159" s="17" t="s">
+        <v>427</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="G159" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5258,7 +5394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D19893C-3433-4E5A-B231-F0E5406405D5}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -5671,10 +5807,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F522EADF-145D-4C25-80A5-C8FF6EE41593}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5977,6 +6113,26 @@
       </c>
       <c r="F15">
         <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>565</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>155</v>
+      </c>
+      <c r="F16">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -5988,8 +6144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C475A255-C3DE-4E6E-A9A6-14E2F40D39D1}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>